<commit_message>
Some Dataset cleaning and analysis
Current progress:
* Graphed some properties of the dataset, inlcuding the heatmap of the different parameters
* Dropped and added some columns, including slice thickness and the pre-treatment case id
* Cleaned imageSubtraction.ipynb to be pretty much redudant to the repo now since it does what other notebooks specialize in

Need to do
* Apply image transformations on these images
* Choose fixed image dimension for all images to put into model
* Analyze and choose which features are important to the underlying goal, predicting progression through RECIST_PostNAC category
</commit_message>
<xml_diff>
--- a/PDAC-Response_CaseIDs_Matched.xlsx
+++ b/PDAC-Response_CaseIDs_Matched.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Surgery\Data\ResearchPrograms\Hepatobiliary\Projects\Fellows Projects\Ahmad B Barekzai\Dr. Wei project\PDAC response\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SimpsonLab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D4FCD27-26F6-409E-A75F-B5208DA595F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B133FBD3-F84E-46AB-B8B9-FDE4DE921641}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{12858033-EE66-468B-B099-9780CFFD60DE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{12858033-EE66-468B-B099-9780CFFD60DE}"/>
   </bookViews>
   <sheets>
     <sheet name="IDs_Matched" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -798,9 +799,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -838,7 +839,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -944,7 +945,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1086,7 +1087,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1100,7 +1101,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomRight" activeCell="S13" sqref="S13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>